<commit_message>
edit inital step for 1 simulation, create player as next step
</commit_message>
<xml_diff>
--- a/data/init/point_harbor.xlsx
+++ b/data/init/point_harbor.xlsx
@@ -5,20 +5,31 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UIUCclass\23SP\IS597PR\FinalProj\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UIUCclass\23SP\IS597PR\FinalProj\2023Spr_projects_catan_simulation\data\init\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B1953E-836C-43AF-A581-EF4F13E6F5A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F086545D-B2D3-448B-BCC5-F2CA3E64BFE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="1980" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3825" yWindow="2820" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -351,7 +362,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="C2" sqref="C2:C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
city prefer, settlement prefer finsihed, harbor prefer in process
</commit_message>
<xml_diff>
--- a/data/init/point_harbor.xlsx
+++ b/data/init/point_harbor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UIUCclass\23SP\IS597PR\FinalProj\2023Spr_projects_catan_simulation\data\init\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F086545D-B2D3-448B-BCC5-F2CA3E64BFE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67870A2B-8925-44AE-94DF-3139BA83507C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3825" yWindow="2820" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,12 +36,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>point</t>
   </si>
   <si>
     <t>harbor</t>
+  </si>
+  <si>
+    <t>harbor_type</t>
+  </si>
+  <si>
+    <t>harbor_resource</t>
   </si>
 </sst>
 </file>
@@ -359,164 +365,278 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C19"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>4</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>6</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>11</v>
       </c>
       <c r="B6">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>16</v>
       </c>
       <c r="B7">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>27</v>
       </c>
       <c r="B8">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>33</v>
       </c>
       <c r="B9">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>43</v>
       </c>
       <c r="B10">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>47</v>
       </c>
       <c r="B11">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>50</v>
       </c>
       <c r="B12">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>53</v>
       </c>
       <c r="B13">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>48</v>
       </c>
       <c r="B14">
         <v>7</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>52</v>
       </c>
       <c r="B15">
         <v>7</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>43</v>
       </c>
       <c r="B16">
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>39</v>
       </c>
       <c r="B17">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>12</v>
       </c>
       <c r="B18">
         <v>9</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="B19">
         <v>9</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>